<commit_message>
do ecxel file fo new tasks
</commit_message>
<xml_diff>
--- a/handlers/materials_for_studying/task_4/task_4.xlsx
+++ b/handlers/materials_for_studying/task_4/task_4.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\george\Desktop\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{9338E5E0-450F-4F05-AD3C-C7DA769B4DD7}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="8_{46E63F51-1347-45F6-BC89-38F87AC86914}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="2880" yWindow="2880" windowWidth="14400" windowHeight="8272" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="6270" yWindow="4170" windowWidth="21600" windowHeight="11385" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Лист1" sheetId="1" r:id="rId1"/>
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="24" uniqueCount="24">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="28" uniqueCount="28">
   <si>
     <t>Верно</t>
   </si>
@@ -106,6 +106,18 @@
   </si>
   <si>
     <t>свеклА</t>
+  </si>
+  <si>
+    <t>дефИс</t>
+  </si>
+  <si>
+    <t>дЕфис</t>
+  </si>
+  <si>
+    <t>лыжнЯ</t>
+  </si>
+  <si>
+    <t>лЫжня</t>
   </si>
 </sst>
 </file>
@@ -437,20 +449,20 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:B12"/>
+  <dimension ref="A1:B14"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B12" sqref="B12"/>
+      <selection activeCell="E5" sqref="E5"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="27.59765625" customWidth="1"/>
-    <col min="2" max="2" width="27.86328125" customWidth="1"/>
-    <col min="3" max="3" width="16.265625" customWidth="1"/>
+    <col min="1" max="1" width="27.5703125" customWidth="1"/>
+    <col min="2" max="2" width="27.85546875" customWidth="1"/>
+    <col min="3" max="3" width="16.28515625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:2" x14ac:dyDescent="0.45">
+    <row r="1" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -458,91 +470,107 @@
         <v>1</v>
       </c>
     </row>
-    <row r="2" spans="1:2" x14ac:dyDescent="0.45">
+    <row r="2" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
+        <v>26</v>
+      </c>
+      <c r="B2" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="3" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A3" t="s">
+        <v>24</v>
+      </c>
+      <c r="B3" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="4" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A4" t="s">
         <v>2</v>
       </c>
-      <c r="B2" t="s">
+      <c r="B4" t="s">
         <v>3</v>
       </c>
     </row>
-    <row r="3" spans="1:2" x14ac:dyDescent="0.45">
-      <c r="A3" t="s">
+    <row r="5" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A5" t="s">
         <v>4</v>
       </c>
-      <c r="B3" t="s">
+      <c r="B5" t="s">
         <v>5</v>
       </c>
     </row>
-    <row r="4" spans="1:2" x14ac:dyDescent="0.45">
-      <c r="A4" t="s">
+    <row r="6" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A6" t="s">
         <v>19</v>
       </c>
-      <c r="B4" t="s">
+      <c r="B6" t="s">
         <v>10</v>
       </c>
     </row>
-    <row r="5" spans="1:2" x14ac:dyDescent="0.45">
-      <c r="A5" t="s">
+    <row r="7" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A7" t="s">
         <v>6</v>
       </c>
-      <c r="B5" t="s">
+      <c r="B7" t="s">
         <v>11</v>
       </c>
     </row>
-    <row r="6" spans="1:2" x14ac:dyDescent="0.45">
-      <c r="A6" t="s">
+    <row r="8" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A8" t="s">
         <v>7</v>
       </c>
-      <c r="B6" t="s">
+      <c r="B8" t="s">
         <v>16</v>
       </c>
     </row>
-    <row r="7" spans="1:2" x14ac:dyDescent="0.45">
-      <c r="A7" t="s">
+    <row r="9" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A9" t="s">
         <v>8</v>
       </c>
-      <c r="B7" t="s">
+      <c r="B9" t="s">
         <v>9</v>
       </c>
     </row>
-    <row r="8" spans="1:2" x14ac:dyDescent="0.45">
-      <c r="A8" t="s">
+    <row r="10" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A10" t="s">
         <v>12</v>
       </c>
-      <c r="B8" t="s">
+      <c r="B10" t="s">
         <v>13</v>
       </c>
     </row>
-    <row r="9" spans="1:2" x14ac:dyDescent="0.45">
-      <c r="A9" t="s">
+    <row r="11" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A11" t="s">
         <v>14</v>
       </c>
-      <c r="B9" t="s">
+      <c r="B11" t="s">
         <v>15</v>
       </c>
     </row>
-    <row r="10" spans="1:2" x14ac:dyDescent="0.45">
-      <c r="A10" t="s">
+    <row r="12" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A12" t="s">
         <v>17</v>
       </c>
-      <c r="B10" t="s">
+      <c r="B12" t="s">
         <v>18</v>
       </c>
     </row>
-    <row r="11" spans="1:2" x14ac:dyDescent="0.45">
-      <c r="A11" t="s">
+    <row r="13" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A13" t="s">
         <v>20</v>
       </c>
-      <c r="B11" t="s">
+      <c r="B13" t="s">
         <v>21</v>
       </c>
     </row>
-    <row r="12" spans="1:2" x14ac:dyDescent="0.45">
-      <c r="A12" t="s">
+    <row r="14" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A14" t="s">
         <v>22</v>
       </c>
-      <c r="B12" t="s">
+      <c r="B14" t="s">
         <v>23</v>
       </c>
     </row>

</xml_diff>

<commit_message>
Chage function to add new tasks
</commit_message>
<xml_diff>
--- a/handlers/materials_for_studying/task_4/task_4.xlsx
+++ b/handlers/materials_for_studying/task_4/task_4.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\george\Desktop\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{D19936D7-E96A-4538-B26E-7B855CC6C827}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="8_{1E9C44F2-B9F8-4A13-9FC1-64C76B79DE1E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="6195" yWindow="3990" windowWidth="21600" windowHeight="11385" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Лист1" sheetId="1" r:id="rId1"/>
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="28" uniqueCount="28">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="30" uniqueCount="30">
   <si>
     <t>Верно</t>
   </si>
@@ -118,6 +118,12 @@
   </si>
   <si>
     <t>лЫжня</t>
+  </si>
+  <si>
+    <t>Илюха крут</t>
+  </si>
+  <si>
+    <t>Илюха лох</t>
   </si>
 </sst>
 </file>
@@ -449,10 +455,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:B16"/>
+  <dimension ref="A1:B15"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C19" sqref="C19"/>
+      <selection activeCell="B16" sqref="B16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -575,19 +581,11 @@
       </c>
     </row>
     <row r="15" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A15">
-        <v>1</v>
-      </c>
-      <c r="B15">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="16" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A16">
-        <v>3</v>
-      </c>
-      <c r="B16">
-        <v>4</v>
+      <c r="A15" t="s">
+        <v>28</v>
+      </c>
+      <c r="B15" t="s">
+        <v>29</v>
       </c>
     </row>
   </sheetData>

</xml_diff>